<commit_message>
Executando validações do 1b
</commit_message>
<xml_diff>
--- a/docs/analise/gpt_5_1/tb_verificar_alteracao_nome_coluna_2025_11_19_base_analise_gpt_5_1.xlsx
+++ b/docs/analise/gpt_5_1/tb_verificar_alteracao_nome_coluna_2025_11_19_base_analise_gpt_5_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="7">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -33,19 +33,32 @@
   <si>
     <t xml:space="preserve">gpt-5.1</t>
   </si>
+  <si>
+    <t xml:space="preserve">positiuvos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total casos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Certos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -105,13 +118,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -237,10 +262,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C386"/>
+  <dimension ref="A1:F386"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,6 +296,13 @@
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E2" s="2" t="n">
+        <f aca="false">SUM(C2:C386)</f>
+        <v>385</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -282,6 +314,12 @@
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>385</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -292,6 +330,13 @@
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <f aca="false">E2/E3</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>